<commit_message>
Make player can't walk to zombie
Edit Levels 5 and 6
</commit_message>
<xml_diff>
--- a/LevelDesign_excel/Level5.xlsx
+++ b/LevelDesign_excel/Level5.xlsx
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AH37" sqref="AH37"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U36" sqref="A1:AF51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,8 +1731,8 @@
       <c r="S12" s="9">
         <v>14</v>
       </c>
-      <c r="T12">
-        <v>0</v>
+      <c r="T12" s="4">
+        <v>9</v>
       </c>
       <c r="U12" s="9">
         <v>14</v>
@@ -1781,44 +1781,44 @@
       <c r="A13" s="13">
         <v>1</v>
       </c>
-      <c r="B13" s="13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="13">
-        <v>1</v>
-      </c>
-      <c r="G13" s="13">
-        <v>1</v>
-      </c>
-      <c r="H13" s="13">
-        <v>1</v>
-      </c>
-      <c r="I13" s="13">
-        <v>1</v>
-      </c>
-      <c r="J13" s="13">
-        <v>1</v>
-      </c>
-      <c r="K13" s="13">
-        <v>1</v>
-      </c>
-      <c r="L13" s="13">
-        <v>1</v>
-      </c>
-      <c r="M13" s="13">
-        <v>1</v>
-      </c>
-      <c r="N13" s="13">
-        <v>1</v>
+      <c r="B13" s="3">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" s="9">
+        <v>14</v>
+      </c>
+      <c r="E13" s="7">
+        <v>5</v>
+      </c>
+      <c r="F13" s="4">
+        <v>9</v>
+      </c>
+      <c r="G13" s="9">
+        <v>14</v>
+      </c>
+      <c r="H13" s="10">
+        <v>7</v>
+      </c>
+      <c r="I13" s="4">
+        <v>9</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="9">
+        <v>14</v>
+      </c>
+      <c r="L13" s="4">
+        <v>9</v>
+      </c>
+      <c r="M13" s="4">
+        <v>9</v>
+      </c>
+      <c r="N13" s="9">
+        <v>14</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -1894,20 +1894,20 @@
       <c r="D14" s="9">
         <v>14</v>
       </c>
-      <c r="E14" s="9">
-        <v>14</v>
-      </c>
-      <c r="F14" s="9">
-        <v>14</v>
+      <c r="E14" s="4">
+        <v>9</v>
+      </c>
+      <c r="F14" s="4">
+        <v>9</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="H14" s="9">
-        <v>14</v>
-      </c>
-      <c r="I14" s="9">
-        <v>14</v>
+      <c r="H14" s="4">
+        <v>9</v>
+      </c>
+      <c r="I14" s="4">
+        <v>9</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -1915,14 +1915,14 @@
       <c r="K14" s="9">
         <v>14</v>
       </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14" s="9">
-        <v>14</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
+      <c r="L14" s="10">
+        <v>7</v>
+      </c>
+      <c r="M14" s="4">
+        <v>9</v>
+      </c>
+      <c r="N14" s="9">
+        <v>14</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -1989,8 +1989,8 @@
       <c r="A15" s="13">
         <v>1</v>
       </c>
-      <c r="B15" s="5">
-        <v>13</v>
+      <c r="B15" s="3">
+        <v>2</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1998,20 +1998,20 @@
       <c r="D15" s="9">
         <v>14</v>
       </c>
-      <c r="E15" s="9">
-        <v>14</v>
-      </c>
-      <c r="F15" s="9">
-        <v>14</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15" s="9">
-        <v>14</v>
-      </c>
-      <c r="I15" s="9">
-        <v>14</v>
+      <c r="E15" s="10">
+        <v>7</v>
+      </c>
+      <c r="F15" s="4">
+        <v>9</v>
+      </c>
+      <c r="G15" s="9">
+        <v>14</v>
+      </c>
+      <c r="H15" s="10">
+        <v>7</v>
+      </c>
+      <c r="I15" s="4">
+        <v>9</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -2019,14 +2019,14 @@
       <c r="K15" s="9">
         <v>14</v>
       </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15" s="9">
-        <v>14</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
+      <c r="L15" s="4">
+        <v>9</v>
+      </c>
+      <c r="M15" s="4">
+        <v>9</v>
+      </c>
+      <c r="N15" s="9">
+        <v>14</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -2304,41 +2304,41 @@
       <c r="B18">
         <v>0</v>
       </c>
-      <c r="C18" s="15">
-        <v>6</v>
-      </c>
-      <c r="D18" s="15">
-        <v>6</v>
-      </c>
-      <c r="E18" s="15">
-        <v>6</v>
-      </c>
-      <c r="F18" s="15">
-        <v>6</v>
-      </c>
-      <c r="G18" s="15">
-        <v>6</v>
-      </c>
-      <c r="H18" s="15">
-        <v>6</v>
-      </c>
-      <c r="I18" s="15">
-        <v>6</v>
-      </c>
-      <c r="J18" s="15">
-        <v>6</v>
-      </c>
-      <c r="K18" s="15">
-        <v>6</v>
-      </c>
-      <c r="L18" s="15">
-        <v>6</v>
-      </c>
-      <c r="M18" s="15">
-        <v>6</v>
-      </c>
-      <c r="N18" s="15">
-        <v>6</v>
+      <c r="C18" s="4">
+        <v>9</v>
+      </c>
+      <c r="D18" s="10">
+        <v>7</v>
+      </c>
+      <c r="E18" s="4">
+        <v>9</v>
+      </c>
+      <c r="F18" s="4">
+        <v>9</v>
+      </c>
+      <c r="G18" s="4">
+        <v>9</v>
+      </c>
+      <c r="H18" s="4">
+        <v>9</v>
+      </c>
+      <c r="I18" s="4">
+        <v>9</v>
+      </c>
+      <c r="J18" s="4">
+        <v>9</v>
+      </c>
+      <c r="K18" s="4">
+        <v>9</v>
+      </c>
+      <c r="L18" s="4">
+        <v>9</v>
+      </c>
+      <c r="M18" s="4">
+        <v>9</v>
+      </c>
+      <c r="N18" s="4">
+        <v>9</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -2405,44 +2405,44 @@
       <c r="A19" s="13">
         <v>1</v>
       </c>
-      <c r="B19" s="12">
-        <v>4</v>
+      <c r="B19" s="4">
+        <v>9</v>
       </c>
       <c r="C19" s="7">
         <v>5</v>
       </c>
-      <c r="D19" s="15">
-        <v>6</v>
-      </c>
-      <c r="E19" s="15">
-        <v>6</v>
-      </c>
-      <c r="F19" s="15">
-        <v>6</v>
-      </c>
-      <c r="G19" s="15">
-        <v>6</v>
-      </c>
-      <c r="H19" s="15">
-        <v>6</v>
-      </c>
-      <c r="I19" s="15">
-        <v>6</v>
-      </c>
-      <c r="J19" s="15">
-        <v>6</v>
-      </c>
-      <c r="K19" s="15">
-        <v>6</v>
-      </c>
-      <c r="L19" s="15">
-        <v>6</v>
-      </c>
-      <c r="M19" s="15">
-        <v>6</v>
-      </c>
-      <c r="N19" s="15">
-        <v>6</v>
+      <c r="D19" s="4">
+        <v>9</v>
+      </c>
+      <c r="E19" s="4">
+        <v>9</v>
+      </c>
+      <c r="F19" s="4">
+        <v>9</v>
+      </c>
+      <c r="G19" s="4">
+        <v>9</v>
+      </c>
+      <c r="H19" s="4">
+        <v>9</v>
+      </c>
+      <c r="I19" s="4">
+        <v>9</v>
+      </c>
+      <c r="J19" s="4">
+        <v>9</v>
+      </c>
+      <c r="K19" s="4">
+        <v>9</v>
+      </c>
+      <c r="L19" s="4">
+        <v>9</v>
+      </c>
+      <c r="M19" s="4">
+        <v>9</v>
+      </c>
+      <c r="N19" s="4">
+        <v>9</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -2503,44 +2503,44 @@
       <c r="A20" s="13">
         <v>1</v>
       </c>
-      <c r="B20" s="12">
-        <v>4</v>
+      <c r="B20" s="4">
+        <v>9</v>
       </c>
       <c r="C20" s="4">
         <v>9</v>
       </c>
-      <c r="D20" s="15">
-        <v>6</v>
-      </c>
-      <c r="E20" s="15">
-        <v>6</v>
-      </c>
-      <c r="F20" s="15">
-        <v>6</v>
-      </c>
-      <c r="G20" s="15">
-        <v>6</v>
-      </c>
-      <c r="H20" s="15">
-        <v>6</v>
-      </c>
-      <c r="I20" s="15">
-        <v>6</v>
-      </c>
-      <c r="J20" s="15">
-        <v>6</v>
-      </c>
-      <c r="K20" s="15">
-        <v>6</v>
-      </c>
-      <c r="L20" s="15">
-        <v>6</v>
-      </c>
-      <c r="M20" s="15">
-        <v>6</v>
-      </c>
-      <c r="N20" s="15">
-        <v>6</v>
+      <c r="D20" s="4">
+        <v>9</v>
+      </c>
+      <c r="E20" s="7">
+        <v>5</v>
+      </c>
+      <c r="F20" s="4">
+        <v>9</v>
+      </c>
+      <c r="G20" s="4">
+        <v>9</v>
+      </c>
+      <c r="H20" s="4">
+        <v>9</v>
+      </c>
+      <c r="I20" s="4">
+        <v>9</v>
+      </c>
+      <c r="J20" s="4">
+        <v>9</v>
+      </c>
+      <c r="K20" s="4">
+        <v>9</v>
+      </c>
+      <c r="L20" s="4">
+        <v>9</v>
+      </c>
+      <c r="M20" s="4">
+        <v>9</v>
+      </c>
+      <c r="N20" s="4">
+        <v>9</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -2601,44 +2601,44 @@
       <c r="A21" s="13">
         <v>1</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="4">
+        <v>9</v>
+      </c>
+      <c r="C21" s="4">
+        <v>9</v>
+      </c>
+      <c r="D21" s="12">
         <v>4</v>
       </c>
-      <c r="C21" s="4">
-        <v>9</v>
-      </c>
-      <c r="D21" s="15">
-        <v>6</v>
-      </c>
-      <c r="E21" s="15">
-        <v>6</v>
-      </c>
-      <c r="F21" s="15">
-        <v>6</v>
-      </c>
-      <c r="G21" s="15">
-        <v>6</v>
-      </c>
-      <c r="H21" s="15">
-        <v>6</v>
-      </c>
-      <c r="I21" s="15">
-        <v>6</v>
-      </c>
-      <c r="J21" s="15">
-        <v>6</v>
-      </c>
-      <c r="K21" s="15">
-        <v>6</v>
-      </c>
-      <c r="L21" s="15">
-        <v>6</v>
-      </c>
-      <c r="M21" s="15">
-        <v>6</v>
-      </c>
-      <c r="N21" s="15">
-        <v>6</v>
+      <c r="E21" s="4">
+        <v>9</v>
+      </c>
+      <c r="F21" s="4">
+        <v>9</v>
+      </c>
+      <c r="G21" s="4">
+        <v>9</v>
+      </c>
+      <c r="H21" s="4">
+        <v>9</v>
+      </c>
+      <c r="I21" s="4">
+        <v>9</v>
+      </c>
+      <c r="J21" s="4">
+        <v>9</v>
+      </c>
+      <c r="K21" s="4">
+        <v>9</v>
+      </c>
+      <c r="L21" s="4">
+        <v>9</v>
+      </c>
+      <c r="M21" s="4">
+        <v>9</v>
+      </c>
+      <c r="N21" s="4">
+        <v>9</v>
       </c>
       <c r="O21">
         <v>0</v>
@@ -2705,38 +2705,38 @@
       <c r="C22" s="4">
         <v>9</v>
       </c>
-      <c r="D22" s="15">
-        <v>6</v>
+      <c r="D22" s="4">
+        <v>9</v>
       </c>
       <c r="E22" s="15">
         <v>6</v>
       </c>
-      <c r="F22" s="15">
-        <v>6</v>
-      </c>
-      <c r="G22" s="15">
-        <v>6</v>
-      </c>
-      <c r="H22" s="15">
-        <v>6</v>
-      </c>
-      <c r="I22" s="15">
-        <v>6</v>
-      </c>
-      <c r="J22" s="15">
-        <v>6</v>
-      </c>
-      <c r="K22" s="15">
-        <v>6</v>
-      </c>
-      <c r="L22" s="15">
-        <v>6</v>
-      </c>
-      <c r="M22" s="15">
-        <v>6</v>
-      </c>
-      <c r="N22" s="15">
-        <v>6</v>
+      <c r="F22" s="4">
+        <v>9</v>
+      </c>
+      <c r="G22" s="4">
+        <v>9</v>
+      </c>
+      <c r="H22" s="4">
+        <v>9</v>
+      </c>
+      <c r="I22" s="4">
+        <v>9</v>
+      </c>
+      <c r="J22" s="4">
+        <v>9</v>
+      </c>
+      <c r="K22" s="4">
+        <v>9</v>
+      </c>
+      <c r="L22" s="4">
+        <v>9</v>
+      </c>
+      <c r="M22" s="4">
+        <v>9</v>
+      </c>
+      <c r="N22" s="4">
+        <v>9</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -2946,8 +2946,8 @@
       <c r="R24">
         <v>0</v>
       </c>
-      <c r="S24">
-        <v>0</v>
+      <c r="S24" s="3">
+        <v>2</v>
       </c>
       <c r="T24" s="13">
         <v>1</v>
@@ -3041,8 +3041,8 @@
       <c r="Q25" s="13">
         <v>1</v>
       </c>
-      <c r="R25" s="13">
-        <v>1</v>
+      <c r="R25" s="12">
+        <v>4</v>
       </c>
       <c r="S25" s="13">
         <v>1</v>
@@ -3094,8 +3094,8 @@
       <c r="B26" s="13">
         <v>1</v>
       </c>
-      <c r="C26">
-        <v>0</v>
+      <c r="C26" s="9">
+        <v>14</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -3103,8 +3103,8 @@
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="F26" s="13">
-        <v>1</v>
+      <c r="F26" s="15">
+        <v>6</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -3216,8 +3216,8 @@
       <c r="J27" s="13">
         <v>1</v>
       </c>
-      <c r="K27" s="13">
-        <v>1</v>
+      <c r="K27" s="12">
+        <v>4</v>
       </c>
       <c r="L27" s="13">
         <v>1</v>
@@ -3314,8 +3314,8 @@
       <c r="J28">
         <v>0</v>
       </c>
-      <c r="K28">
-        <v>0</v>
+      <c r="K28" s="4">
+        <v>9</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -3332,8 +3332,8 @@
       <c r="P28" s="13">
         <v>1</v>
       </c>
-      <c r="Q28">
-        <v>0</v>
+      <c r="Q28" s="3">
+        <v>2</v>
       </c>
       <c r="R28" s="13">
         <v>1</v>
@@ -3412,8 +3412,8 @@
       <c r="J29" s="13">
         <v>1</v>
       </c>
-      <c r="K29" s="13">
-        <v>1</v>
+      <c r="K29" s="12">
+        <v>4</v>
       </c>
       <c r="L29" s="13">
         <v>1</v>
@@ -3682,11 +3682,11 @@
       <c r="B32" s="13">
         <v>1</v>
       </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
+      <c r="C32" s="3">
+        <v>2</v>
+      </c>
+      <c r="D32" s="4">
+        <v>9</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -3700,14 +3700,14 @@
       <c r="H32" s="13">
         <v>1</v>
       </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
+      <c r="I32" s="9">
+        <v>14</v>
+      </c>
+      <c r="J32" s="4">
+        <v>9</v>
+      </c>
+      <c r="K32" s="9">
+        <v>14</v>
       </c>
       <c r="L32" s="13">
         <v>1</v>
@@ -3926,8 +3926,8 @@
       <c r="R34" s="13">
         <v>1</v>
       </c>
-      <c r="S34">
-        <v>0</v>
+      <c r="S34" s="3">
+        <v>2</v>
       </c>
       <c r="T34" s="13">
         <v>1</v>
@@ -4000,8 +4000,8 @@
       <c r="J35" s="13">
         <v>1</v>
       </c>
-      <c r="K35">
-        <v>0</v>
+      <c r="K35" s="9">
+        <v>14</v>
       </c>
       <c r="L35" s="13">
         <v>1</v>
@@ -4104,8 +4104,8 @@
       <c r="L36" s="13">
         <v>1</v>
       </c>
-      <c r="M36">
-        <v>0</v>
+      <c r="M36" s="9">
+        <v>14</v>
       </c>
       <c r="N36">
         <v>0</v>
@@ -4113,17 +4113,17 @@
       <c r="O36">
         <v>0</v>
       </c>
-      <c r="P36">
-        <v>0</v>
-      </c>
-      <c r="Q36">
-        <v>0</v>
-      </c>
-      <c r="R36">
-        <v>0</v>
-      </c>
-      <c r="S36">
-        <v>0</v>
+      <c r="P36" s="9">
+        <v>14</v>
+      </c>
+      <c r="Q36" s="4">
+        <v>9</v>
+      </c>
+      <c r="R36" s="9">
+        <v>14</v>
+      </c>
+      <c r="S36" s="9">
+        <v>14</v>
       </c>
       <c r="T36" s="13">
         <v>1</v>
@@ -4202,8 +4202,8 @@
       <c r="L37" s="13">
         <v>1</v>
       </c>
-      <c r="M37">
-        <v>0</v>
+      <c r="M37" s="4">
+        <v>9</v>
       </c>
       <c r="N37" s="13">
         <v>1</v>
@@ -4270,14 +4270,14 @@
       <c r="B38" s="13">
         <v>1</v>
       </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
+      <c r="C38" s="10">
+        <v>7</v>
+      </c>
+      <c r="D38" s="4">
+        <v>9</v>
+      </c>
+      <c r="E38" s="3">
+        <v>2</v>
       </c>
       <c r="F38" s="13">
         <v>1</v>
@@ -4294,14 +4294,14 @@
       <c r="J38" s="13">
         <v>1</v>
       </c>
-      <c r="K38">
-        <v>0</v>
+      <c r="K38" s="9">
+        <v>14</v>
       </c>
       <c r="L38">
         <v>0</v>
       </c>
-      <c r="M38">
-        <v>0</v>
+      <c r="M38" s="9">
+        <v>14</v>
       </c>
       <c r="N38" s="13">
         <v>1</v>
@@ -4318,8 +4318,8 @@
       <c r="R38" s="13">
         <v>1</v>
       </c>
-      <c r="S38">
-        <v>0</v>
+      <c r="S38" s="9">
+        <v>14</v>
       </c>
       <c r="T38" s="13">
         <v>1</v>
@@ -4368,8 +4368,8 @@
       <c r="B39" s="13">
         <v>1</v>
       </c>
-      <c r="C39">
-        <v>0</v>
+      <c r="C39" s="4">
+        <v>9</v>
       </c>
       <c r="D39" s="13">
         <v>1</v>
@@ -4392,8 +4392,8 @@
       <c r="J39" s="13">
         <v>1</v>
       </c>
-      <c r="K39" s="13">
-        <v>1</v>
+      <c r="K39" s="7">
+        <v>5</v>
       </c>
       <c r="L39" s="13">
         <v>1</v>
@@ -4416,8 +4416,8 @@
       <c r="R39" s="13">
         <v>1</v>
       </c>
-      <c r="S39">
-        <v>0</v>
+      <c r="S39" s="9">
+        <v>14</v>
       </c>
       <c r="T39" s="13">
         <v>1</v>
@@ -4514,8 +4514,8 @@
       <c r="R40" s="13">
         <v>1</v>
       </c>
-      <c r="S40">
-        <v>0</v>
+      <c r="S40" s="9">
+        <v>14</v>
       </c>
       <c r="T40">
         <v>0</v>
@@ -4618,35 +4618,35 @@
       <c r="T41" s="13">
         <v>1</v>
       </c>
-      <c r="U41">
-        <v>0</v>
-      </c>
-      <c r="V41">
-        <v>0</v>
-      </c>
-      <c r="W41">
-        <v>0</v>
-      </c>
-      <c r="X41">
-        <v>0</v>
-      </c>
-      <c r="Y41">
-        <v>0</v>
-      </c>
-      <c r="Z41">
-        <v>0</v>
-      </c>
-      <c r="AA41">
-        <v>0</v>
-      </c>
-      <c r="AB41">
-        <v>0</v>
-      </c>
-      <c r="AC41">
-        <v>0</v>
-      </c>
-      <c r="AD41">
-        <v>0</v>
+      <c r="U41" s="13">
+        <v>1</v>
+      </c>
+      <c r="V41" s="13">
+        <v>1</v>
+      </c>
+      <c r="W41" s="13">
+        <v>1</v>
+      </c>
+      <c r="X41" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y41" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA41" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB41" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC41" s="13">
+        <v>1</v>
+      </c>
+      <c r="AD41" s="13">
+        <v>1</v>
       </c>
       <c r="AE41">
         <v>0</v>
@@ -4689,11 +4689,11 @@
       <c r="K42">
         <v>0</v>
       </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-      <c r="M42">
-        <v>0</v>
+      <c r="L42" s="3">
+        <v>2</v>
+      </c>
+      <c r="M42" s="4">
+        <v>9</v>
       </c>
       <c r="N42">
         <v>0</v>
@@ -4707,11 +4707,11 @@
       <c r="Q42">
         <v>0</v>
       </c>
-      <c r="R42">
-        <v>0</v>
-      </c>
-      <c r="S42">
-        <v>0</v>
+      <c r="R42" s="4">
+        <v>9</v>
+      </c>
+      <c r="S42" s="3">
+        <v>2</v>
       </c>
       <c r="T42">
         <v>0</v>
@@ -4725,26 +4725,26 @@
       <c r="W42">
         <v>0</v>
       </c>
-      <c r="X42">
-        <v>0</v>
-      </c>
-      <c r="Y42">
-        <v>0</v>
+      <c r="X42" s="9">
+        <v>14</v>
+      </c>
+      <c r="Y42" s="9">
+        <v>14</v>
       </c>
       <c r="Z42">
         <v>0</v>
       </c>
-      <c r="AA42">
-        <v>0</v>
-      </c>
-      <c r="AB42">
-        <v>0</v>
+      <c r="AA42" s="9">
+        <v>14</v>
+      </c>
+      <c r="AB42" s="9">
+        <v>14</v>
       </c>
       <c r="AC42">
         <v>0</v>
       </c>
-      <c r="AD42">
-        <v>0</v>
+      <c r="AD42" s="13">
+        <v>1</v>
       </c>
       <c r="AE42">
         <v>0</v>
@@ -4778,62 +4778,62 @@
       <c r="H43" s="13">
         <v>1</v>
       </c>
-      <c r="I43" s="12">
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43" s="13">
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43" s="13">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43" s="13">
+        <v>1</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43" s="13">
+        <v>1</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43" s="13">
+        <v>1</v>
+      </c>
+      <c r="S43">
+        <v>0</v>
+      </c>
+      <c r="T43" s="13">
+        <v>1</v>
+      </c>
+      <c r="U43">
+        <v>0</v>
+      </c>
+      <c r="V43" s="13">
+        <v>1</v>
+      </c>
+      <c r="W43" s="13">
+        <v>1</v>
+      </c>
+      <c r="X43" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y43" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z43" s="12">
         <v>4</v>
       </c>
-      <c r="J43" s="13">
-        <v>1</v>
-      </c>
-      <c r="K43" s="3">
-        <v>2</v>
-      </c>
-      <c r="L43" s="13">
-        <v>1</v>
-      </c>
-      <c r="M43">
-        <v>0</v>
-      </c>
-      <c r="N43" s="13">
-        <v>1</v>
-      </c>
-      <c r="O43">
-        <v>0</v>
-      </c>
-      <c r="P43" s="13">
-        <v>1</v>
-      </c>
-      <c r="Q43">
-        <v>0</v>
-      </c>
-      <c r="R43" s="13">
-        <v>1</v>
-      </c>
-      <c r="S43">
-        <v>0</v>
-      </c>
-      <c r="T43" s="13">
-        <v>1</v>
-      </c>
-      <c r="U43">
-        <v>0</v>
-      </c>
-      <c r="V43" s="13">
-        <v>1</v>
-      </c>
-      <c r="W43" s="4">
-        <v>9</v>
-      </c>
-      <c r="X43" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y43">
-        <v>0</v>
-      </c>
-      <c r="Z43" s="13">
-        <v>1</v>
-      </c>
-      <c r="AA43">
-        <v>0</v>
+      <c r="AA43" s="13">
+        <v>1</v>
       </c>
       <c r="AB43" s="13">
         <v>1</v>
@@ -4867,77 +4867,77 @@
       <c r="E44">
         <v>0</v>
       </c>
-      <c r="F44" s="13">
-        <v>1</v>
-      </c>
-      <c r="G44" s="2">
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44" s="9">
+        <v>14</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44" s="2">
         <v>30</v>
       </c>
-      <c r="H44" s="13">
-        <v>1</v>
-      </c>
-      <c r="I44" s="4">
-        <v>9</v>
-      </c>
-      <c r="J44" s="13">
-        <v>1</v>
-      </c>
-      <c r="K44">
-        <v>0</v>
-      </c>
-      <c r="L44" s="13">
-        <v>1</v>
+      <c r="L44">
+        <v>0</v>
       </c>
       <c r="M44">
         <v>0</v>
       </c>
-      <c r="N44" s="13">
-        <v>1</v>
+      <c r="N44">
+        <v>0</v>
       </c>
       <c r="O44">
         <v>0</v>
       </c>
-      <c r="P44" s="13">
-        <v>1</v>
-      </c>
-      <c r="Q44" s="2">
-        <v>30</v>
-      </c>
-      <c r="R44" s="13">
-        <v>1</v>
-      </c>
-      <c r="S44">
-        <v>0</v>
-      </c>
-      <c r="T44" s="13">
-        <v>1</v>
-      </c>
-      <c r="U44" s="9">
-        <v>14</v>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <v>0</v>
+      </c>
+      <c r="S44" s="9">
+        <v>14</v>
+      </c>
+      <c r="T44">
+        <v>0</v>
+      </c>
+      <c r="U44">
+        <v>0</v>
       </c>
       <c r="V44" s="13">
         <v>1</v>
       </c>
-      <c r="W44" s="4">
-        <v>9</v>
-      </c>
-      <c r="X44" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y44">
-        <v>0</v>
-      </c>
-      <c r="Z44" s="13">
-        <v>1</v>
-      </c>
-      <c r="AA44">
-        <v>0</v>
-      </c>
-      <c r="AB44" s="13">
-        <v>1</v>
-      </c>
-      <c r="AC44">
-        <v>0</v>
+      <c r="W44" s="9">
+        <v>14</v>
+      </c>
+      <c r="X44" s="9">
+        <v>14</v>
+      </c>
+      <c r="Y44" s="9">
+        <v>14</v>
+      </c>
+      <c r="Z44">
+        <v>0</v>
+      </c>
+      <c r="AA44" s="9">
+        <v>14</v>
+      </c>
+      <c r="AB44" s="9">
+        <v>14</v>
+      </c>
+      <c r="AC44" s="9">
+        <v>14</v>
       </c>
       <c r="AD44" s="13">
         <v>1</v>
@@ -4974,8 +4974,8 @@
       <c r="H45" s="13">
         <v>1</v>
       </c>
-      <c r="I45" s="4">
-        <v>9</v>
+      <c r="I45">
+        <v>0</v>
       </c>
       <c r="J45" s="13">
         <v>1</v>
@@ -5016,26 +5016,26 @@
       <c r="V45" s="13">
         <v>1</v>
       </c>
-      <c r="W45" s="4">
-        <v>9</v>
+      <c r="W45">
+        <v>0</v>
       </c>
       <c r="X45" s="13">
         <v>1</v>
       </c>
-      <c r="Y45">
-        <v>0</v>
-      </c>
-      <c r="Z45" s="13">
-        <v>1</v>
-      </c>
-      <c r="AA45">
-        <v>0</v>
+      <c r="Y45" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z45" s="12">
+        <v>4</v>
+      </c>
+      <c r="AA45" s="13">
+        <v>1</v>
       </c>
       <c r="AB45" s="13">
         <v>1</v>
       </c>
-      <c r="AC45">
-        <v>0</v>
+      <c r="AC45" s="13">
+        <v>1</v>
       </c>
       <c r="AD45" s="13">
         <v>1</v>
@@ -5066,8 +5066,8 @@
       <c r="F46">
         <v>0</v>
       </c>
-      <c r="G46" s="10">
-        <v>7</v>
+      <c r="G46" s="2">
+        <v>30</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -5078,65 +5078,65 @@
       <c r="J46">
         <v>0</v>
       </c>
-      <c r="K46" s="4">
-        <v>9</v>
+      <c r="K46" s="9">
+        <v>14</v>
       </c>
       <c r="L46">
         <v>0</v>
       </c>
-      <c r="M46" s="2">
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46" s="9">
+        <v>14</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="S46" s="2">
         <v>30</v>
       </c>
-      <c r="N46">
-        <v>0</v>
-      </c>
-      <c r="O46">
-        <v>0</v>
-      </c>
-      <c r="P46">
-        <v>0</v>
-      </c>
-      <c r="Q46" s="3">
-        <v>2</v>
-      </c>
-      <c r="R46">
-        <v>0</v>
-      </c>
-      <c r="S46">
-        <v>0</v>
-      </c>
-      <c r="T46" s="15">
-        <v>6</v>
+      <c r="T46" s="4">
+        <v>9</v>
       </c>
       <c r="U46">
         <v>0</v>
       </c>
-      <c r="V46">
-        <v>0</v>
-      </c>
-      <c r="W46" s="12">
-        <v>4</v>
-      </c>
-      <c r="X46">
-        <v>0</v>
-      </c>
-      <c r="Y46">
-        <v>0</v>
-      </c>
-      <c r="Z46" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA46">
-        <v>0</v>
-      </c>
-      <c r="AB46">
-        <v>0</v>
-      </c>
-      <c r="AC46" s="2">
-        <v>30</v>
-      </c>
-      <c r="AD46">
-        <v>0</v>
+      <c r="V46" s="13">
+        <v>1</v>
+      </c>
+      <c r="W46">
+        <v>0</v>
+      </c>
+      <c r="X46" s="9">
+        <v>14</v>
+      </c>
+      <c r="Y46" s="9">
+        <v>14</v>
+      </c>
+      <c r="Z46">
+        <v>0</v>
+      </c>
+      <c r="AA46" s="9">
+        <v>14</v>
+      </c>
+      <c r="AB46" s="9">
+        <v>14</v>
+      </c>
+      <c r="AC46">
+        <v>0</v>
+      </c>
+      <c r="AD46" s="13">
+        <v>1</v>
       </c>
       <c r="AE46">
         <v>0</v>
@@ -5158,8 +5158,8 @@
       <c r="D47" s="13">
         <v>1</v>
       </c>
-      <c r="E47">
-        <v>0</v>
+      <c r="E47" s="3">
+        <v>2</v>
       </c>
       <c r="F47" s="13">
         <v>1</v>
@@ -5212,20 +5212,20 @@
       <c r="V47" s="13">
         <v>1</v>
       </c>
-      <c r="W47">
-        <v>0</v>
+      <c r="W47" s="12">
+        <v>4</v>
       </c>
       <c r="X47" s="13">
         <v>1</v>
       </c>
-      <c r="Y47">
-        <v>0</v>
-      </c>
-      <c r="Z47" s="13">
-        <v>1</v>
-      </c>
-      <c r="AA47">
-        <v>0</v>
+      <c r="Y47" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z47" s="12">
+        <v>4</v>
+      </c>
+      <c r="AA47" s="13">
+        <v>1</v>
       </c>
       <c r="AB47" s="13">
         <v>1</v>
@@ -5259,50 +5259,50 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48" s="13">
-        <v>1</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48" s="13">
-        <v>1</v>
-      </c>
-      <c r="I48" s="9">
-        <v>14</v>
-      </c>
-      <c r="J48" s="13">
-        <v>1</v>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48" s="9">
+        <v>14</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
       </c>
       <c r="K48">
         <v>0</v>
       </c>
-      <c r="L48" s="13">
-        <v>1</v>
+      <c r="L48">
+        <v>0</v>
       </c>
       <c r="M48">
         <v>0</v>
       </c>
-      <c r="N48" s="13">
-        <v>1</v>
-      </c>
-      <c r="O48">
-        <v>0</v>
-      </c>
-      <c r="P48" s="13">
-        <v>1</v>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48" s="2">
+        <v>30</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
       </c>
       <c r="Q48">
         <v>0</v>
       </c>
-      <c r="R48" s="13">
-        <v>1</v>
-      </c>
-      <c r="S48">
-        <v>0</v>
-      </c>
-      <c r="T48" s="13">
-        <v>1</v>
+      <c r="R48">
+        <v>0</v>
+      </c>
+      <c r="S48" s="9">
+        <v>14</v>
+      </c>
+      <c r="T48">
+        <v>0</v>
       </c>
       <c r="U48">
         <v>0</v>
@@ -5310,26 +5310,26 @@
       <c r="V48" s="13">
         <v>1</v>
       </c>
-      <c r="W48" s="2">
-        <v>30</v>
-      </c>
-      <c r="X48" s="13">
-        <v>1</v>
+      <c r="W48">
+        <v>0</v>
+      </c>
+      <c r="X48" s="9">
+        <v>14</v>
       </c>
       <c r="Y48">
         <v>0</v>
       </c>
-      <c r="Z48" s="13">
-        <v>1</v>
+      <c r="Z48" s="9">
+        <v>14</v>
       </c>
       <c r="AA48">
         <v>0</v>
       </c>
-      <c r="AB48" s="13">
-        <v>1</v>
-      </c>
-      <c r="AC48" s="9">
-        <v>14</v>
+      <c r="AB48" s="9">
+        <v>14</v>
+      </c>
+      <c r="AC48">
+        <v>0</v>
       </c>
       <c r="AD48" s="13">
         <v>1</v>
@@ -5372,8 +5372,8 @@
       <c r="J49" s="13">
         <v>1</v>
       </c>
-      <c r="K49">
-        <v>0</v>
+      <c r="K49" s="7">
+        <v>5</v>
       </c>
       <c r="L49" s="13">
         <v>1</v>
@@ -5414,20 +5414,20 @@
       <c r="X49" s="13">
         <v>1</v>
       </c>
-      <c r="Y49">
-        <v>0</v>
+      <c r="Y49" s="12">
+        <v>4</v>
       </c>
       <c r="Z49" s="13">
         <v>1</v>
       </c>
-      <c r="AA49">
-        <v>0</v>
+      <c r="AA49" s="12">
+        <v>4</v>
       </c>
       <c r="AB49" s="13">
         <v>1</v>
       </c>
-      <c r="AC49">
-        <v>0</v>
+      <c r="AC49" s="12">
+        <v>4</v>
       </c>
       <c r="AD49" s="13">
         <v>1</v>
@@ -5470,8 +5470,8 @@
       <c r="J50">
         <v>0</v>
       </c>
-      <c r="K50">
-        <v>0</v>
+      <c r="K50" s="3">
+        <v>2</v>
       </c>
       <c r="L50">
         <v>0</v>
@@ -5482,8 +5482,8 @@
       <c r="N50">
         <v>0</v>
       </c>
-      <c r="O50">
-        <v>0</v>
+      <c r="O50" s="12">
+        <v>4</v>
       </c>
       <c r="P50">
         <v>0</v>
@@ -5503,14 +5503,14 @@
       <c r="U50">
         <v>0</v>
       </c>
-      <c r="V50">
-        <v>0</v>
+      <c r="V50" s="13">
+        <v>1</v>
       </c>
       <c r="W50">
         <v>0</v>
       </c>
-      <c r="X50">
-        <v>0</v>
+      <c r="X50" s="9">
+        <v>14</v>
       </c>
       <c r="Y50">
         <v>0</v>
@@ -5521,8 +5521,8 @@
       <c r="AA50">
         <v>0</v>
       </c>
-      <c r="AB50">
-        <v>0</v>
+      <c r="AB50" s="9">
+        <v>14</v>
       </c>
       <c r="AC50">
         <v>0</v>

</xml_diff>

<commit_message>
added lv3 and fixed some stuff
</commit_message>
<xml_diff>
--- a/LevelDesign_excel/Level5.xlsx
+++ b/LevelDesign_excel/Level5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SP3_Grp3\LevelDesign_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shing\Desktop\SP3_Grp3\LevelDesign_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AH37" sqref="AH37"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AE18" sqref="AE18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +524,8 @@
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="32" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="31" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.28515625" customWidth="1"/>
     <col min="43" max="43" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="45" max="47" width="2.7109375" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Change Back levels 5 and 6 excel to new one
</commit_message>
<xml_diff>
--- a/LevelDesign_excel/Level5.xlsx
+++ b/LevelDesign_excel/Level5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shing\Desktop\SP3_Grp3\LevelDesign_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SP3_Grp3\LevelDesign_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AE18" sqref="AE18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U36" sqref="A1:AF51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,8 +524,7 @@
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="31" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4.28515625" customWidth="1"/>
+    <col min="4" max="32" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="45" max="47" width="2.7109375" bestFit="1" customWidth="1"/>
@@ -1732,8 +1731,8 @@
       <c r="S12" s="9">
         <v>14</v>
       </c>
-      <c r="T12">
-        <v>0</v>
+      <c r="T12" s="4">
+        <v>9</v>
       </c>
       <c r="U12" s="9">
         <v>14</v>
@@ -1782,44 +1781,44 @@
       <c r="A13" s="13">
         <v>1</v>
       </c>
-      <c r="B13" s="13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="13">
-        <v>1</v>
-      </c>
-      <c r="G13" s="13">
-        <v>1</v>
-      </c>
-      <c r="H13" s="13">
-        <v>1</v>
-      </c>
-      <c r="I13" s="13">
-        <v>1</v>
-      </c>
-      <c r="J13" s="13">
-        <v>1</v>
-      </c>
-      <c r="K13" s="13">
-        <v>1</v>
-      </c>
-      <c r="L13" s="13">
-        <v>1</v>
-      </c>
-      <c r="M13" s="13">
-        <v>1</v>
-      </c>
-      <c r="N13" s="13">
-        <v>1</v>
+      <c r="B13" s="3">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" s="9">
+        <v>14</v>
+      </c>
+      <c r="E13" s="7">
+        <v>5</v>
+      </c>
+      <c r="F13" s="4">
+        <v>9</v>
+      </c>
+      <c r="G13" s="9">
+        <v>14</v>
+      </c>
+      <c r="H13" s="10">
+        <v>7</v>
+      </c>
+      <c r="I13" s="4">
+        <v>9</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="9">
+        <v>14</v>
+      </c>
+      <c r="L13" s="4">
+        <v>9</v>
+      </c>
+      <c r="M13" s="4">
+        <v>9</v>
+      </c>
+      <c r="N13" s="9">
+        <v>14</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -1895,20 +1894,20 @@
       <c r="D14" s="9">
         <v>14</v>
       </c>
-      <c r="E14" s="9">
-        <v>14</v>
-      </c>
-      <c r="F14" s="9">
-        <v>14</v>
+      <c r="E14" s="4">
+        <v>9</v>
+      </c>
+      <c r="F14" s="4">
+        <v>9</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="H14" s="9">
-        <v>14</v>
-      </c>
-      <c r="I14" s="9">
-        <v>14</v>
+      <c r="H14" s="4">
+        <v>9</v>
+      </c>
+      <c r="I14" s="4">
+        <v>9</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -1916,14 +1915,14 @@
       <c r="K14" s="9">
         <v>14</v>
       </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14" s="9">
-        <v>14</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
+      <c r="L14" s="10">
+        <v>7</v>
+      </c>
+      <c r="M14" s="4">
+        <v>9</v>
+      </c>
+      <c r="N14" s="9">
+        <v>14</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -1990,8 +1989,8 @@
       <c r="A15" s="13">
         <v>1</v>
       </c>
-      <c r="B15" s="5">
-        <v>13</v>
+      <c r="B15" s="3">
+        <v>2</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1999,20 +1998,20 @@
       <c r="D15" s="9">
         <v>14</v>
       </c>
-      <c r="E15" s="9">
-        <v>14</v>
-      </c>
-      <c r="F15" s="9">
-        <v>14</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15" s="9">
-        <v>14</v>
-      </c>
-      <c r="I15" s="9">
-        <v>14</v>
+      <c r="E15" s="10">
+        <v>7</v>
+      </c>
+      <c r="F15" s="4">
+        <v>9</v>
+      </c>
+      <c r="G15" s="9">
+        <v>14</v>
+      </c>
+      <c r="H15" s="10">
+        <v>7</v>
+      </c>
+      <c r="I15" s="4">
+        <v>9</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -2020,14 +2019,14 @@
       <c r="K15" s="9">
         <v>14</v>
       </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15" s="9">
-        <v>14</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
+      <c r="L15" s="4">
+        <v>9</v>
+      </c>
+      <c r="M15" s="4">
+        <v>9</v>
+      </c>
+      <c r="N15" s="9">
+        <v>14</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -2305,41 +2304,41 @@
       <c r="B18">
         <v>0</v>
       </c>
-      <c r="C18" s="15">
-        <v>6</v>
-      </c>
-      <c r="D18" s="15">
-        <v>6</v>
-      </c>
-      <c r="E18" s="15">
-        <v>6</v>
-      </c>
-      <c r="F18" s="15">
-        <v>6</v>
-      </c>
-      <c r="G18" s="15">
-        <v>6</v>
-      </c>
-      <c r="H18" s="15">
-        <v>6</v>
-      </c>
-      <c r="I18" s="15">
-        <v>6</v>
-      </c>
-      <c r="J18" s="15">
-        <v>6</v>
-      </c>
-      <c r="K18" s="15">
-        <v>6</v>
-      </c>
-      <c r="L18" s="15">
-        <v>6</v>
-      </c>
-      <c r="M18" s="15">
-        <v>6</v>
-      </c>
-      <c r="N18" s="15">
-        <v>6</v>
+      <c r="C18" s="4">
+        <v>9</v>
+      </c>
+      <c r="D18" s="10">
+        <v>7</v>
+      </c>
+      <c r="E18" s="4">
+        <v>9</v>
+      </c>
+      <c r="F18" s="4">
+        <v>9</v>
+      </c>
+      <c r="G18" s="4">
+        <v>9</v>
+      </c>
+      <c r="H18" s="4">
+        <v>9</v>
+      </c>
+      <c r="I18" s="4">
+        <v>9</v>
+      </c>
+      <c r="J18" s="4">
+        <v>9</v>
+      </c>
+      <c r="K18" s="4">
+        <v>9</v>
+      </c>
+      <c r="L18" s="4">
+        <v>9</v>
+      </c>
+      <c r="M18" s="4">
+        <v>9</v>
+      </c>
+      <c r="N18" s="4">
+        <v>9</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -2406,44 +2405,44 @@
       <c r="A19" s="13">
         <v>1</v>
       </c>
-      <c r="B19" s="12">
-        <v>4</v>
+      <c r="B19" s="4">
+        <v>9</v>
       </c>
       <c r="C19" s="7">
         <v>5</v>
       </c>
-      <c r="D19" s="15">
-        <v>6</v>
-      </c>
-      <c r="E19" s="15">
-        <v>6</v>
-      </c>
-      <c r="F19" s="15">
-        <v>6</v>
-      </c>
-      <c r="G19" s="15">
-        <v>6</v>
-      </c>
-      <c r="H19" s="15">
-        <v>6</v>
-      </c>
-      <c r="I19" s="15">
-        <v>6</v>
-      </c>
-      <c r="J19" s="15">
-        <v>6</v>
-      </c>
-      <c r="K19" s="15">
-        <v>6</v>
-      </c>
-      <c r="L19" s="15">
-        <v>6</v>
-      </c>
-      <c r="M19" s="15">
-        <v>6</v>
-      </c>
-      <c r="N19" s="15">
-        <v>6</v>
+      <c r="D19" s="4">
+        <v>9</v>
+      </c>
+      <c r="E19" s="4">
+        <v>9</v>
+      </c>
+      <c r="F19" s="4">
+        <v>9</v>
+      </c>
+      <c r="G19" s="4">
+        <v>9</v>
+      </c>
+      <c r="H19" s="4">
+        <v>9</v>
+      </c>
+      <c r="I19" s="4">
+        <v>9</v>
+      </c>
+      <c r="J19" s="4">
+        <v>9</v>
+      </c>
+      <c r="K19" s="4">
+        <v>9</v>
+      </c>
+      <c r="L19" s="4">
+        <v>9</v>
+      </c>
+      <c r="M19" s="4">
+        <v>9</v>
+      </c>
+      <c r="N19" s="4">
+        <v>9</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -2504,44 +2503,44 @@
       <c r="A20" s="13">
         <v>1</v>
       </c>
-      <c r="B20" s="12">
-        <v>4</v>
+      <c r="B20" s="4">
+        <v>9</v>
       </c>
       <c r="C20" s="4">
         <v>9</v>
       </c>
-      <c r="D20" s="15">
-        <v>6</v>
-      </c>
-      <c r="E20" s="15">
-        <v>6</v>
-      </c>
-      <c r="F20" s="15">
-        <v>6</v>
-      </c>
-      <c r="G20" s="15">
-        <v>6</v>
-      </c>
-      <c r="H20" s="15">
-        <v>6</v>
-      </c>
-      <c r="I20" s="15">
-        <v>6</v>
-      </c>
-      <c r="J20" s="15">
-        <v>6</v>
-      </c>
-      <c r="K20" s="15">
-        <v>6</v>
-      </c>
-      <c r="L20" s="15">
-        <v>6</v>
-      </c>
-      <c r="M20" s="15">
-        <v>6</v>
-      </c>
-      <c r="N20" s="15">
-        <v>6</v>
+      <c r="D20" s="4">
+        <v>9</v>
+      </c>
+      <c r="E20" s="7">
+        <v>5</v>
+      </c>
+      <c r="F20" s="4">
+        <v>9</v>
+      </c>
+      <c r="G20" s="4">
+        <v>9</v>
+      </c>
+      <c r="H20" s="4">
+        <v>9</v>
+      </c>
+      <c r="I20" s="4">
+        <v>9</v>
+      </c>
+      <c r="J20" s="4">
+        <v>9</v>
+      </c>
+      <c r="K20" s="4">
+        <v>9</v>
+      </c>
+      <c r="L20" s="4">
+        <v>9</v>
+      </c>
+      <c r="M20" s="4">
+        <v>9</v>
+      </c>
+      <c r="N20" s="4">
+        <v>9</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -2602,44 +2601,44 @@
       <c r="A21" s="13">
         <v>1</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="4">
+        <v>9</v>
+      </c>
+      <c r="C21" s="4">
+        <v>9</v>
+      </c>
+      <c r="D21" s="12">
         <v>4</v>
       </c>
-      <c r="C21" s="4">
-        <v>9</v>
-      </c>
-      <c r="D21" s="15">
-        <v>6</v>
-      </c>
-      <c r="E21" s="15">
-        <v>6</v>
-      </c>
-      <c r="F21" s="15">
-        <v>6</v>
-      </c>
-      <c r="G21" s="15">
-        <v>6</v>
-      </c>
-      <c r="H21" s="15">
-        <v>6</v>
-      </c>
-      <c r="I21" s="15">
-        <v>6</v>
-      </c>
-      <c r="J21" s="15">
-        <v>6</v>
-      </c>
-      <c r="K21" s="15">
-        <v>6</v>
-      </c>
-      <c r="L21" s="15">
-        <v>6</v>
-      </c>
-      <c r="M21" s="15">
-        <v>6</v>
-      </c>
-      <c r="N21" s="15">
-        <v>6</v>
+      <c r="E21" s="4">
+        <v>9</v>
+      </c>
+      <c r="F21" s="4">
+        <v>9</v>
+      </c>
+      <c r="G21" s="4">
+        <v>9</v>
+      </c>
+      <c r="H21" s="4">
+        <v>9</v>
+      </c>
+      <c r="I21" s="4">
+        <v>9</v>
+      </c>
+      <c r="J21" s="4">
+        <v>9</v>
+      </c>
+      <c r="K21" s="4">
+        <v>9</v>
+      </c>
+      <c r="L21" s="4">
+        <v>9</v>
+      </c>
+      <c r="M21" s="4">
+        <v>9</v>
+      </c>
+      <c r="N21" s="4">
+        <v>9</v>
       </c>
       <c r="O21">
         <v>0</v>
@@ -2706,38 +2705,38 @@
       <c r="C22" s="4">
         <v>9</v>
       </c>
-      <c r="D22" s="15">
-        <v>6</v>
+      <c r="D22" s="4">
+        <v>9</v>
       </c>
       <c r="E22" s="15">
         <v>6</v>
       </c>
-      <c r="F22" s="15">
-        <v>6</v>
-      </c>
-      <c r="G22" s="15">
-        <v>6</v>
-      </c>
-      <c r="H22" s="15">
-        <v>6</v>
-      </c>
-      <c r="I22" s="15">
-        <v>6</v>
-      </c>
-      <c r="J22" s="15">
-        <v>6</v>
-      </c>
-      <c r="K22" s="15">
-        <v>6</v>
-      </c>
-      <c r="L22" s="15">
-        <v>6</v>
-      </c>
-      <c r="M22" s="15">
-        <v>6</v>
-      </c>
-      <c r="N22" s="15">
-        <v>6</v>
+      <c r="F22" s="4">
+        <v>9</v>
+      </c>
+      <c r="G22" s="4">
+        <v>9</v>
+      </c>
+      <c r="H22" s="4">
+        <v>9</v>
+      </c>
+      <c r="I22" s="4">
+        <v>9</v>
+      </c>
+      <c r="J22" s="4">
+        <v>9</v>
+      </c>
+      <c r="K22" s="4">
+        <v>9</v>
+      </c>
+      <c r="L22" s="4">
+        <v>9</v>
+      </c>
+      <c r="M22" s="4">
+        <v>9</v>
+      </c>
+      <c r="N22" s="4">
+        <v>9</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -2947,8 +2946,8 @@
       <c r="R24">
         <v>0</v>
       </c>
-      <c r="S24">
-        <v>0</v>
+      <c r="S24" s="3">
+        <v>2</v>
       </c>
       <c r="T24" s="13">
         <v>1</v>
@@ -3042,8 +3041,8 @@
       <c r="Q25" s="13">
         <v>1</v>
       </c>
-      <c r="R25" s="13">
-        <v>1</v>
+      <c r="R25" s="12">
+        <v>4</v>
       </c>
       <c r="S25" s="13">
         <v>1</v>
@@ -3095,8 +3094,8 @@
       <c r="B26" s="13">
         <v>1</v>
       </c>
-      <c r="C26">
-        <v>0</v>
+      <c r="C26" s="9">
+        <v>14</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -3104,8 +3103,8 @@
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="F26" s="13">
-        <v>1</v>
+      <c r="F26" s="15">
+        <v>6</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -3217,8 +3216,8 @@
       <c r="J27" s="13">
         <v>1</v>
       </c>
-      <c r="K27" s="13">
-        <v>1</v>
+      <c r="K27" s="12">
+        <v>4</v>
       </c>
       <c r="L27" s="13">
         <v>1</v>
@@ -3315,8 +3314,8 @@
       <c r="J28">
         <v>0</v>
       </c>
-      <c r="K28">
-        <v>0</v>
+      <c r="K28" s="4">
+        <v>9</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -3333,8 +3332,8 @@
       <c r="P28" s="13">
         <v>1</v>
       </c>
-      <c r="Q28">
-        <v>0</v>
+      <c r="Q28" s="3">
+        <v>2</v>
       </c>
       <c r="R28" s="13">
         <v>1</v>
@@ -3413,8 +3412,8 @@
       <c r="J29" s="13">
         <v>1</v>
       </c>
-      <c r="K29" s="13">
-        <v>1</v>
+      <c r="K29" s="12">
+        <v>4</v>
       </c>
       <c r="L29" s="13">
         <v>1</v>
@@ -3683,11 +3682,11 @@
       <c r="B32" s="13">
         <v>1</v>
       </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
+      <c r="C32" s="3">
+        <v>2</v>
+      </c>
+      <c r="D32" s="4">
+        <v>9</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -3701,14 +3700,14 @@
       <c r="H32" s="13">
         <v>1</v>
       </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
+      <c r="I32" s="9">
+        <v>14</v>
+      </c>
+      <c r="J32" s="4">
+        <v>9</v>
+      </c>
+      <c r="K32" s="9">
+        <v>14</v>
       </c>
       <c r="L32" s="13">
         <v>1</v>
@@ -3927,8 +3926,8 @@
       <c r="R34" s="13">
         <v>1</v>
       </c>
-      <c r="S34">
-        <v>0</v>
+      <c r="S34" s="3">
+        <v>2</v>
       </c>
       <c r="T34" s="13">
         <v>1</v>
@@ -4001,8 +4000,8 @@
       <c r="J35" s="13">
         <v>1</v>
       </c>
-      <c r="K35">
-        <v>0</v>
+      <c r="K35" s="9">
+        <v>14</v>
       </c>
       <c r="L35" s="13">
         <v>1</v>
@@ -4105,8 +4104,8 @@
       <c r="L36" s="13">
         <v>1</v>
       </c>
-      <c r="M36">
-        <v>0</v>
+      <c r="M36" s="9">
+        <v>14</v>
       </c>
       <c r="N36">
         <v>0</v>
@@ -4114,17 +4113,17 @@
       <c r="O36">
         <v>0</v>
       </c>
-      <c r="P36">
-        <v>0</v>
-      </c>
-      <c r="Q36">
-        <v>0</v>
-      </c>
-      <c r="R36">
-        <v>0</v>
-      </c>
-      <c r="S36">
-        <v>0</v>
+      <c r="P36" s="9">
+        <v>14</v>
+      </c>
+      <c r="Q36" s="4">
+        <v>9</v>
+      </c>
+      <c r="R36" s="9">
+        <v>14</v>
+      </c>
+      <c r="S36" s="9">
+        <v>14</v>
       </c>
       <c r="T36" s="13">
         <v>1</v>
@@ -4203,8 +4202,8 @@
       <c r="L37" s="13">
         <v>1</v>
       </c>
-      <c r="M37">
-        <v>0</v>
+      <c r="M37" s="4">
+        <v>9</v>
       </c>
       <c r="N37" s="13">
         <v>1</v>
@@ -4271,14 +4270,14 @@
       <c r="B38" s="13">
         <v>1</v>
       </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
+      <c r="C38" s="10">
+        <v>7</v>
+      </c>
+      <c r="D38" s="4">
+        <v>9</v>
+      </c>
+      <c r="E38" s="3">
+        <v>2</v>
       </c>
       <c r="F38" s="13">
         <v>1</v>
@@ -4295,14 +4294,14 @@
       <c r="J38" s="13">
         <v>1</v>
       </c>
-      <c r="K38">
-        <v>0</v>
+      <c r="K38" s="9">
+        <v>14</v>
       </c>
       <c r="L38">
         <v>0</v>
       </c>
-      <c r="M38">
-        <v>0</v>
+      <c r="M38" s="9">
+        <v>14</v>
       </c>
       <c r="N38" s="13">
         <v>1</v>
@@ -4319,8 +4318,8 @@
       <c r="R38" s="13">
         <v>1</v>
       </c>
-      <c r="S38">
-        <v>0</v>
+      <c r="S38" s="9">
+        <v>14</v>
       </c>
       <c r="T38" s="13">
         <v>1</v>
@@ -4369,8 +4368,8 @@
       <c r="B39" s="13">
         <v>1</v>
       </c>
-      <c r="C39">
-        <v>0</v>
+      <c r="C39" s="4">
+        <v>9</v>
       </c>
       <c r="D39" s="13">
         <v>1</v>
@@ -4393,8 +4392,8 @@
       <c r="J39" s="13">
         <v>1</v>
       </c>
-      <c r="K39" s="13">
-        <v>1</v>
+      <c r="K39" s="7">
+        <v>5</v>
       </c>
       <c r="L39" s="13">
         <v>1</v>
@@ -4417,8 +4416,8 @@
       <c r="R39" s="13">
         <v>1</v>
       </c>
-      <c r="S39">
-        <v>0</v>
+      <c r="S39" s="9">
+        <v>14</v>
       </c>
       <c r="T39" s="13">
         <v>1</v>
@@ -4515,8 +4514,8 @@
       <c r="R40" s="13">
         <v>1</v>
       </c>
-      <c r="S40">
-        <v>0</v>
+      <c r="S40" s="9">
+        <v>14</v>
       </c>
       <c r="T40">
         <v>0</v>
@@ -4619,35 +4618,35 @@
       <c r="T41" s="13">
         <v>1</v>
       </c>
-      <c r="U41">
-        <v>0</v>
-      </c>
-      <c r="V41">
-        <v>0</v>
-      </c>
-      <c r="W41">
-        <v>0</v>
-      </c>
-      <c r="X41">
-        <v>0</v>
-      </c>
-      <c r="Y41">
-        <v>0</v>
-      </c>
-      <c r="Z41">
-        <v>0</v>
-      </c>
-      <c r="AA41">
-        <v>0</v>
-      </c>
-      <c r="AB41">
-        <v>0</v>
-      </c>
-      <c r="AC41">
-        <v>0</v>
-      </c>
-      <c r="AD41">
-        <v>0</v>
+      <c r="U41" s="13">
+        <v>1</v>
+      </c>
+      <c r="V41" s="13">
+        <v>1</v>
+      </c>
+      <c r="W41" s="13">
+        <v>1</v>
+      </c>
+      <c r="X41" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y41" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA41" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB41" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC41" s="13">
+        <v>1</v>
+      </c>
+      <c r="AD41" s="13">
+        <v>1</v>
       </c>
       <c r="AE41">
         <v>0</v>
@@ -4690,11 +4689,11 @@
       <c r="K42">
         <v>0</v>
       </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-      <c r="M42">
-        <v>0</v>
+      <c r="L42" s="3">
+        <v>2</v>
+      </c>
+      <c r="M42" s="4">
+        <v>9</v>
       </c>
       <c r="N42">
         <v>0</v>
@@ -4708,11 +4707,11 @@
       <c r="Q42">
         <v>0</v>
       </c>
-      <c r="R42">
-        <v>0</v>
-      </c>
-      <c r="S42">
-        <v>0</v>
+      <c r="R42" s="4">
+        <v>9</v>
+      </c>
+      <c r="S42" s="3">
+        <v>2</v>
       </c>
       <c r="T42">
         <v>0</v>
@@ -4726,26 +4725,26 @@
       <c r="W42">
         <v>0</v>
       </c>
-      <c r="X42">
-        <v>0</v>
-      </c>
-      <c r="Y42">
-        <v>0</v>
+      <c r="X42" s="9">
+        <v>14</v>
+      </c>
+      <c r="Y42" s="9">
+        <v>14</v>
       </c>
       <c r="Z42">
         <v>0</v>
       </c>
-      <c r="AA42">
-        <v>0</v>
-      </c>
-      <c r="AB42">
-        <v>0</v>
+      <c r="AA42" s="9">
+        <v>14</v>
+      </c>
+      <c r="AB42" s="9">
+        <v>14</v>
       </c>
       <c r="AC42">
         <v>0</v>
       </c>
-      <c r="AD42">
-        <v>0</v>
+      <c r="AD42" s="13">
+        <v>1</v>
       </c>
       <c r="AE42">
         <v>0</v>
@@ -4779,62 +4778,62 @@
       <c r="H43" s="13">
         <v>1</v>
       </c>
-      <c r="I43" s="12">
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43" s="13">
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43" s="13">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43" s="13">
+        <v>1</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43" s="13">
+        <v>1</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43" s="13">
+        <v>1</v>
+      </c>
+      <c r="S43">
+        <v>0</v>
+      </c>
+      <c r="T43" s="13">
+        <v>1</v>
+      </c>
+      <c r="U43">
+        <v>0</v>
+      </c>
+      <c r="V43" s="13">
+        <v>1</v>
+      </c>
+      <c r="W43" s="13">
+        <v>1</v>
+      </c>
+      <c r="X43" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y43" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z43" s="12">
         <v>4</v>
       </c>
-      <c r="J43" s="13">
-        <v>1</v>
-      </c>
-      <c r="K43" s="3">
-        <v>2</v>
-      </c>
-      <c r="L43" s="13">
-        <v>1</v>
-      </c>
-      <c r="M43">
-        <v>0</v>
-      </c>
-      <c r="N43" s="13">
-        <v>1</v>
-      </c>
-      <c r="O43">
-        <v>0</v>
-      </c>
-      <c r="P43" s="13">
-        <v>1</v>
-      </c>
-      <c r="Q43">
-        <v>0</v>
-      </c>
-      <c r="R43" s="13">
-        <v>1</v>
-      </c>
-      <c r="S43">
-        <v>0</v>
-      </c>
-      <c r="T43" s="13">
-        <v>1</v>
-      </c>
-      <c r="U43">
-        <v>0</v>
-      </c>
-      <c r="V43" s="13">
-        <v>1</v>
-      </c>
-      <c r="W43" s="4">
-        <v>9</v>
-      </c>
-      <c r="X43" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y43">
-        <v>0</v>
-      </c>
-      <c r="Z43" s="13">
-        <v>1</v>
-      </c>
-      <c r="AA43">
-        <v>0</v>
+      <c r="AA43" s="13">
+        <v>1</v>
       </c>
       <c r="AB43" s="13">
         <v>1</v>
@@ -4868,77 +4867,77 @@
       <c r="E44">
         <v>0</v>
       </c>
-      <c r="F44" s="13">
-        <v>1</v>
-      </c>
-      <c r="G44" s="2">
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44" s="9">
+        <v>14</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44" s="2">
         <v>30</v>
       </c>
-      <c r="H44" s="13">
-        <v>1</v>
-      </c>
-      <c r="I44" s="4">
-        <v>9</v>
-      </c>
-      <c r="J44" s="13">
-        <v>1</v>
-      </c>
-      <c r="K44">
-        <v>0</v>
-      </c>
-      <c r="L44" s="13">
-        <v>1</v>
+      <c r="L44">
+        <v>0</v>
       </c>
       <c r="M44">
         <v>0</v>
       </c>
-      <c r="N44" s="13">
-        <v>1</v>
+      <c r="N44">
+        <v>0</v>
       </c>
       <c r="O44">
         <v>0</v>
       </c>
-      <c r="P44" s="13">
-        <v>1</v>
-      </c>
-      <c r="Q44" s="2">
-        <v>30</v>
-      </c>
-      <c r="R44" s="13">
-        <v>1</v>
-      </c>
-      <c r="S44">
-        <v>0</v>
-      </c>
-      <c r="T44" s="13">
-        <v>1</v>
-      </c>
-      <c r="U44" s="9">
-        <v>14</v>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <v>0</v>
+      </c>
+      <c r="S44" s="9">
+        <v>14</v>
+      </c>
+      <c r="T44">
+        <v>0</v>
+      </c>
+      <c r="U44">
+        <v>0</v>
       </c>
       <c r="V44" s="13">
         <v>1</v>
       </c>
-      <c r="W44" s="4">
-        <v>9</v>
-      </c>
-      <c r="X44" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y44">
-        <v>0</v>
-      </c>
-      <c r="Z44" s="13">
-        <v>1</v>
-      </c>
-      <c r="AA44">
-        <v>0</v>
-      </c>
-      <c r="AB44" s="13">
-        <v>1</v>
-      </c>
-      <c r="AC44">
-        <v>0</v>
+      <c r="W44" s="9">
+        <v>14</v>
+      </c>
+      <c r="X44" s="9">
+        <v>14</v>
+      </c>
+      <c r="Y44" s="9">
+        <v>14</v>
+      </c>
+      <c r="Z44">
+        <v>0</v>
+      </c>
+      <c r="AA44" s="9">
+        <v>14</v>
+      </c>
+      <c r="AB44" s="9">
+        <v>14</v>
+      </c>
+      <c r="AC44" s="9">
+        <v>14</v>
       </c>
       <c r="AD44" s="13">
         <v>1</v>
@@ -4975,8 +4974,8 @@
       <c r="H45" s="13">
         <v>1</v>
       </c>
-      <c r="I45" s="4">
-        <v>9</v>
+      <c r="I45">
+        <v>0</v>
       </c>
       <c r="J45" s="13">
         <v>1</v>
@@ -5017,26 +5016,26 @@
       <c r="V45" s="13">
         <v>1</v>
       </c>
-      <c r="W45" s="4">
-        <v>9</v>
+      <c r="W45">
+        <v>0</v>
       </c>
       <c r="X45" s="13">
         <v>1</v>
       </c>
-      <c r="Y45">
-        <v>0</v>
-      </c>
-      <c r="Z45" s="13">
-        <v>1</v>
-      </c>
-      <c r="AA45">
-        <v>0</v>
+      <c r="Y45" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z45" s="12">
+        <v>4</v>
+      </c>
+      <c r="AA45" s="13">
+        <v>1</v>
       </c>
       <c r="AB45" s="13">
         <v>1</v>
       </c>
-      <c r="AC45">
-        <v>0</v>
+      <c r="AC45" s="13">
+        <v>1</v>
       </c>
       <c r="AD45" s="13">
         <v>1</v>
@@ -5067,8 +5066,8 @@
       <c r="F46">
         <v>0</v>
       </c>
-      <c r="G46" s="10">
-        <v>7</v>
+      <c r="G46" s="2">
+        <v>30</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -5079,65 +5078,65 @@
       <c r="J46">
         <v>0</v>
       </c>
-      <c r="K46" s="4">
-        <v>9</v>
+      <c r="K46" s="9">
+        <v>14</v>
       </c>
       <c r="L46">
         <v>0</v>
       </c>
-      <c r="M46" s="2">
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46" s="9">
+        <v>14</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="S46" s="2">
         <v>30</v>
       </c>
-      <c r="N46">
-        <v>0</v>
-      </c>
-      <c r="O46">
-        <v>0</v>
-      </c>
-      <c r="P46">
-        <v>0</v>
-      </c>
-      <c r="Q46" s="3">
-        <v>2</v>
-      </c>
-      <c r="R46">
-        <v>0</v>
-      </c>
-      <c r="S46">
-        <v>0</v>
-      </c>
-      <c r="T46" s="15">
-        <v>6</v>
+      <c r="T46" s="4">
+        <v>9</v>
       </c>
       <c r="U46">
         <v>0</v>
       </c>
-      <c r="V46">
-        <v>0</v>
-      </c>
-      <c r="W46" s="12">
-        <v>4</v>
-      </c>
-      <c r="X46">
-        <v>0</v>
-      </c>
-      <c r="Y46">
-        <v>0</v>
-      </c>
-      <c r="Z46" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA46">
-        <v>0</v>
-      </c>
-      <c r="AB46">
-        <v>0</v>
-      </c>
-      <c r="AC46" s="2">
-        <v>30</v>
-      </c>
-      <c r="AD46">
-        <v>0</v>
+      <c r="V46" s="13">
+        <v>1</v>
+      </c>
+      <c r="W46">
+        <v>0</v>
+      </c>
+      <c r="X46" s="9">
+        <v>14</v>
+      </c>
+      <c r="Y46" s="9">
+        <v>14</v>
+      </c>
+      <c r="Z46">
+        <v>0</v>
+      </c>
+      <c r="AA46" s="9">
+        <v>14</v>
+      </c>
+      <c r="AB46" s="9">
+        <v>14</v>
+      </c>
+      <c r="AC46">
+        <v>0</v>
+      </c>
+      <c r="AD46" s="13">
+        <v>1</v>
       </c>
       <c r="AE46">
         <v>0</v>
@@ -5159,8 +5158,8 @@
       <c r="D47" s="13">
         <v>1</v>
       </c>
-      <c r="E47">
-        <v>0</v>
+      <c r="E47" s="3">
+        <v>2</v>
       </c>
       <c r="F47" s="13">
         <v>1</v>
@@ -5213,20 +5212,20 @@
       <c r="V47" s="13">
         <v>1</v>
       </c>
-      <c r="W47">
-        <v>0</v>
+      <c r="W47" s="12">
+        <v>4</v>
       </c>
       <c r="X47" s="13">
         <v>1</v>
       </c>
-      <c r="Y47">
-        <v>0</v>
-      </c>
-      <c r="Z47" s="13">
-        <v>1</v>
-      </c>
-      <c r="AA47">
-        <v>0</v>
+      <c r="Y47" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z47" s="12">
+        <v>4</v>
+      </c>
+      <c r="AA47" s="13">
+        <v>1</v>
       </c>
       <c r="AB47" s="13">
         <v>1</v>
@@ -5260,50 +5259,50 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48" s="13">
-        <v>1</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48" s="13">
-        <v>1</v>
-      </c>
-      <c r="I48" s="9">
-        <v>14</v>
-      </c>
-      <c r="J48" s="13">
-        <v>1</v>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48" s="9">
+        <v>14</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
       </c>
       <c r="K48">
         <v>0</v>
       </c>
-      <c r="L48" s="13">
-        <v>1</v>
+      <c r="L48">
+        <v>0</v>
       </c>
       <c r="M48">
         <v>0</v>
       </c>
-      <c r="N48" s="13">
-        <v>1</v>
-      </c>
-      <c r="O48">
-        <v>0</v>
-      </c>
-      <c r="P48" s="13">
-        <v>1</v>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48" s="2">
+        <v>30</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
       </c>
       <c r="Q48">
         <v>0</v>
       </c>
-      <c r="R48" s="13">
-        <v>1</v>
-      </c>
-      <c r="S48">
-        <v>0</v>
-      </c>
-      <c r="T48" s="13">
-        <v>1</v>
+      <c r="R48">
+        <v>0</v>
+      </c>
+      <c r="S48" s="9">
+        <v>14</v>
+      </c>
+      <c r="T48">
+        <v>0</v>
       </c>
       <c r="U48">
         <v>0</v>
@@ -5311,26 +5310,26 @@
       <c r="V48" s="13">
         <v>1</v>
       </c>
-      <c r="W48" s="2">
-        <v>30</v>
-      </c>
-      <c r="X48" s="13">
-        <v>1</v>
+      <c r="W48">
+        <v>0</v>
+      </c>
+      <c r="X48" s="9">
+        <v>14</v>
       </c>
       <c r="Y48">
         <v>0</v>
       </c>
-      <c r="Z48" s="13">
-        <v>1</v>
+      <c r="Z48" s="9">
+        <v>14</v>
       </c>
       <c r="AA48">
         <v>0</v>
       </c>
-      <c r="AB48" s="13">
-        <v>1</v>
-      </c>
-      <c r="AC48" s="9">
-        <v>14</v>
+      <c r="AB48" s="9">
+        <v>14</v>
+      </c>
+      <c r="AC48">
+        <v>0</v>
       </c>
       <c r="AD48" s="13">
         <v>1</v>
@@ -5373,8 +5372,8 @@
       <c r="J49" s="13">
         <v>1</v>
       </c>
-      <c r="K49">
-        <v>0</v>
+      <c r="K49" s="7">
+        <v>5</v>
       </c>
       <c r="L49" s="13">
         <v>1</v>
@@ -5415,20 +5414,20 @@
       <c r="X49" s="13">
         <v>1</v>
       </c>
-      <c r="Y49">
-        <v>0</v>
+      <c r="Y49" s="12">
+        <v>4</v>
       </c>
       <c r="Z49" s="13">
         <v>1</v>
       </c>
-      <c r="AA49">
-        <v>0</v>
+      <c r="AA49" s="12">
+        <v>4</v>
       </c>
       <c r="AB49" s="13">
         <v>1</v>
       </c>
-      <c r="AC49">
-        <v>0</v>
+      <c r="AC49" s="12">
+        <v>4</v>
       </c>
       <c r="AD49" s="13">
         <v>1</v>
@@ -5471,8 +5470,8 @@
       <c r="J50">
         <v>0</v>
       </c>
-      <c r="K50">
-        <v>0</v>
+      <c r="K50" s="3">
+        <v>2</v>
       </c>
       <c r="L50">
         <v>0</v>
@@ -5483,8 +5482,8 @@
       <c r="N50">
         <v>0</v>
       </c>
-      <c r="O50">
-        <v>0</v>
+      <c r="O50" s="12">
+        <v>4</v>
       </c>
       <c r="P50">
         <v>0</v>
@@ -5504,14 +5503,14 @@
       <c r="U50">
         <v>0</v>
       </c>
-      <c r="V50">
-        <v>0</v>
+      <c r="V50" s="13">
+        <v>1</v>
       </c>
       <c r="W50">
         <v>0</v>
       </c>
-      <c r="X50">
-        <v>0</v>
+      <c r="X50" s="9">
+        <v>14</v>
       </c>
       <c r="Y50">
         <v>0</v>
@@ -5522,8 +5521,8 @@
       <c r="AA50">
         <v>0</v>
       </c>
-      <c r="AB50">
-        <v>0</v>
+      <c r="AB50" s="9">
+        <v>14</v>
       </c>
       <c r="AC50">
         <v>0</v>

</xml_diff>